<commit_message>
literacy 0308 -> 0309
</commit_message>
<xml_diff>
--- a/data/quiz0516.xlsx
+++ b/data/quiz0516.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="249">
   <si>
     <t>과목명 : 생활속의통계학-01(005036)</t>
   </si>
@@ -796,6 +796,10 @@
   </si>
   <si>
     <t>Red</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ss</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1237,7 +1241,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N66"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A42" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" workbookViewId="0">
       <selection activeCell="A60" sqref="A60:XFD60"/>
     </sheetView>
   </sheetViews>
@@ -3568,8 +3572,8 @@
       </c>
     </row>
     <row r="60" spans="1:14" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="10">
-        <v>58</v>
+      <c r="A60" s="10" t="s">
+        <v>248</v>
       </c>
       <c r="B60" s="11"/>
       <c r="C60" s="10" t="s">

</xml_diff>